<commit_message>
Updated Sprint Backlog, 64% completed!
</commit_message>
<xml_diff>
--- a/Documents/CSE_360_Sprint_Backlog.xlsx
+++ b/Documents/CSE_360_Sprint_Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d873ca24adebd211/Documents/GitHub/CSE360Team11GroupProject/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chetd\OneDrive\Documents\GitHub\CSE360Team11GroupProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -457,6 +457,15 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -467,9 +476,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="12"/>
         <color auto="1"/>
-        <name val="Arial"/>
+        <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -493,15 +502,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -512,9 +512,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color auto="1"/>
-        <name val="Times New Roman"/>
+        <name val="Arial"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -574,18 +574,18 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:G24"/>
-  <sortState ref="A2:G23">
-    <sortCondition ref="A2:A23" customList="High,Medium,Low"/>
-    <sortCondition ref="E2:E23" customList="In Progress,Not Started,Done"/>
+  <sortState ref="A2:G24">
+    <sortCondition ref="E2:E24" customList="In Progress,Not Started,Done"/>
+    <sortCondition ref="A2:A24" customList="High,Medium,Low,Reach"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Priority" dataDxfId="8"/>
-    <tableColumn id="7" name="Task ID" dataDxfId="2"/>
-    <tableColumn id="2" name="Task" dataDxfId="7"/>
-    <tableColumn id="6" name="Dependencies" dataDxfId="3"/>
-    <tableColumn id="3" name="Status" dataDxfId="6"/>
-    <tableColumn id="4" name="Time Spent(days)" dataDxfId="5"/>
-    <tableColumn id="5" name="Owner" dataDxfId="4"/>
+    <tableColumn id="7" name="Task ID" dataDxfId="7"/>
+    <tableColumn id="2" name="Task" dataDxfId="6"/>
+    <tableColumn id="6" name="Dependencies" dataDxfId="5"/>
+    <tableColumn id="3" name="Status" dataDxfId="4"/>
+    <tableColumn id="4" name="Time Spent(days)" dataDxfId="3"/>
+    <tableColumn id="5" name="Owner" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -916,26 +916,26 @@
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" ht="16.149999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="7" t="s">
-        <v>19</v>
+      <c r="A2" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="7">
-        <v>21</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
@@ -951,30 +951,30 @@
     </row>
     <row r="3" spans="1:13" ht="16.149999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B3" s="7">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="17">
         <f>K3/J3</f>
-        <v>0.54545454545454541</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="J3" s="18">
         <f>COUNT(B2:B23)</f>
@@ -982,109 +982,109 @@
       </c>
       <c r="K3" s="19">
         <f>COUNTIF(Table4[Status],"Done")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
-        <v>19</v>
+      <c r="A4" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>10</v>
+        <v>56</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="7">
-        <v>7</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="4"/>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
+      <c r="A5" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="7">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>6</v>
+        <v>57</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="4"/>
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="7">
         <v>19</v>
       </c>
-      <c r="B6" s="7">
-        <v>3</v>
-      </c>
       <c r="C6" s="10" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1"/>
       <c r="J6" s="4"/>
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A7" s="7" t="s">
-        <v>19</v>
+      <c r="A7" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="7">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="4"/>
@@ -1092,154 +1092,154 @@
     </row>
     <row r="8" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7">
-        <v>2</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="4"/>
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="7">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>55</v>
+      <c r="A9" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="12">
+        <v>22</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="7">
-        <v>14</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>42</v>
+        <v>7</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="H9" s="1"/>
       <c r="J9" s="4"/>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="7">
-        <v>2</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>43</v>
+        <v>21</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="4"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A11" s="8" t="s">
-        <v>31</v>
+      <c r="A11" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H11" s="1"/>
       <c r="J11" s="4"/>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A12" s="8" t="s">
-        <v>31</v>
+      <c r="A12" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="7">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="7">
-        <v>4</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="H12" s="1"/>
       <c r="J12" s="4"/>
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A13" s="8" t="s">
-        <v>31</v>
+      <c r="A13" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B13" s="7">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="7">
-        <v>14</v>
-      </c>
-      <c r="G13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="1"/>
@@ -1247,26 +1247,26 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A14" s="8" t="s">
-        <v>31</v>
+      <c r="A14" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B14" s="7">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>8</v>
+        <v>49</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="H14" s="1"/>
       <c r="J14" s="4"/>
@@ -1274,13 +1274,13 @@
     </row>
     <row r="15" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B15" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>50</v>
@@ -1300,25 +1300,25 @@
     </row>
     <row r="16" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B16" s="7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="7">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="1"/>
       <c r="J16" s="4"/>
@@ -1326,13 +1326,13 @@
     </row>
     <row r="17" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B17" s="7">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>52</v>
@@ -1344,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1"/>
       <c r="J17" s="4"/>
@@ -1355,10 +1355,10 @@
         <v>31</v>
       </c>
       <c r="B18" s="7">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>52</v>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="F18" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H18" s="1"/>
       <c r="J18" s="4"/>
@@ -1381,22 +1381,22 @@
         <v>31</v>
       </c>
       <c r="B19" s="7">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="H19" s="1"/>
       <c r="J19" s="4"/>
@@ -1404,25 +1404,25 @@
     </row>
     <row r="20" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B20" s="7">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="H20" s="1"/>
       <c r="J20" s="4"/>
@@ -1430,25 +1430,25 @@
     </row>
     <row r="21" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B21" s="7">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="F21" s="7">
+        <v>2</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H21" s="1"/>
       <c r="J21" s="4"/>
@@ -1456,51 +1456,51 @@
     </row>
     <row r="22" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B22" s="7">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H22" s="1"/>
       <c r="J22" s="4"/>
       <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="12">
-        <v>22</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>63</v>
+      <c r="A23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="7">
+        <v>15</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="H23" s="1"/>
       <c r="J23" s="4"/>

</xml_diff>

<commit_message>
Update from group meeting
This counts for everyone. GJ
</commit_message>
<xml_diff>
--- a/Documents/CSE_360_Sprint_Backlog.xlsx
+++ b/Documents/CSE_360_Sprint_Backlog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Chet</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
   </si>
   <si>
     <t>Task ID: 7</t>
-  </si>
-  <si>
-    <t>Task ID: 5</t>
   </si>
   <si>
     <t>Task ID: All other tasks</t>
@@ -219,7 +213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -280,6 +274,12 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -381,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -418,6 +418,9 @@
     <xf numFmtId="9" fontId="9" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +602,7 @@
   </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" name="Total" dataDxfId="1">
-      <calculatedColumnFormula>COUNT(B2:B23)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNT(B2:B22)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="# Done" dataDxfId="0">
       <calculatedColumnFormula>COUNTIF(Table4[Status],"Done")</calculatedColumnFormula>
@@ -874,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -891,22 +894,22 @@
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
@@ -917,96 +920,96 @@
     </row>
     <row r="2" spans="1:13" ht="16.149999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="7">
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="15" t="s">
-        <v>29</v>
-      </c>
       <c r="K2" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="16.149999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7">
         <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" s="7">
         <v>4</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="17">
         <f>K3/J3</f>
-        <v>0.63636363636363635</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="J3" s="18">
-        <f>COUNT(B2:B23)</f>
-        <v>22</v>
+        <f>COUNT(B2:B22)</f>
+        <v>21</v>
       </c>
       <c r="K3" s="19">
         <f>COUNTIF(Table4[Status],"Done")</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="7">
         <v>17</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="7">
         <v>14</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="4"/>
@@ -1014,51 +1017,51 @@
     </row>
     <row r="5" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="7">
         <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>11</v>
+        <v>56</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="9">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="H6" s="1"/>
       <c r="J6" s="4"/>
@@ -1066,77 +1069,77 @@
     </row>
     <row r="7" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="7">
         <v>20</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="4"/>
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="7">
-        <v>21</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>62</v>
+      <c r="A8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="12">
+        <v>22</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="4"/>
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="12">
-        <v>22</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>63</v>
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="F9" s="7">
+        <v>21</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="H9" s="1"/>
       <c r="J9" s="4"/>
@@ -1144,25 +1147,25 @@
     </row>
     <row r="10" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>10</v>
+        <v>46</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="F10" s="7">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="4"/>
@@ -1170,25 +1173,25 @@
     </row>
     <row r="11" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="7">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="F11" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1"/>
       <c r="J11" s="4"/>
@@ -1196,25 +1199,25 @@
     </row>
     <row r="12" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="7">
+        <v>3</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H12" s="1"/>
       <c r="J12" s="4"/>
@@ -1222,51 +1225,51 @@
     </row>
     <row r="13" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="4"/>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A14" s="7" t="s">
-        <v>19</v>
+      <c r="A14" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B14" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="7">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="H14" s="1"/>
       <c r="J14" s="4"/>
@@ -1274,25 +1277,25 @@
     </row>
     <row r="15" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="7">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H15" s="1"/>
       <c r="J15" s="4"/>
@@ -1300,22 +1303,22 @@
     </row>
     <row r="16" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="7">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>42</v>
@@ -1326,22 +1329,22 @@
     </row>
     <row r="17" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B17" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>43</v>
@@ -1352,25 +1355,25 @@
     </row>
     <row r="18" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="7">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="H18" s="1"/>
       <c r="J18" s="4"/>
@@ -1378,25 +1381,25 @@
     </row>
     <row r="19" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="7">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" s="7">
         <v>2</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="H19" s="1"/>
       <c r="J19" s="4"/>
@@ -1404,25 +1407,25 @@
     </row>
     <row r="20" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="7">
         <v>2</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H20" s="1"/>
       <c r="J20" s="4"/>
@@ -1430,25 +1433,25 @@
     </row>
     <row r="21" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="7">
         <v>2</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H21" s="1"/>
       <c r="J21" s="4"/>
@@ -1456,22 +1459,22 @@
     </row>
     <row r="22" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="7">
+        <v>15</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>52</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>42</v>
@@ -1480,53 +1483,46 @@
       <c r="J22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A23" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="7">
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="7">
-        <v>1</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="J23" s="4"/>
-      <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="D23" s="11"/>
+      <c r="E23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="J23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.4" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="G24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="J24" s="5"/>
-      <c r="M24" s="5"/>
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Updated backlog to show sound as "done"
</commit_message>
<xml_diff>
--- a/Documents/CSE_360_Sprint_Backlog.xlsx
+++ b/Documents/CSE_360_Sprint_Backlog.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collinkofroth/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chet\OneDrive\Documents\GitHub\CSE360Team11GroupProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="23060" windowHeight="11880"/>
+    <workbookView xWindow="360" yWindow="465" windowWidth="23055" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>Task</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Create Use Case Scenarios</t>
@@ -583,8 +580,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:G24"/>
   <sortState ref="A2:G24">
-    <sortCondition ref="E2:E24" customList="In Progress,Not Started,Done"/>
-    <sortCondition ref="A2:A24" customList="High,Medium,Low,Reach"/>
+    <sortCondition ref="A1:A24" customList="High,Medium,Low,Reach"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Priority" dataDxfId="8"/>
@@ -607,7 +603,7 @@
   </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" name="Total" dataDxfId="1">
-      <calculatedColumnFormula>COUNT(B2:B22)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNT(B2:B21)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="# Done" dataDxfId="0">
       <calculatedColumnFormula>COUNTIF(Table4[Status],"Done")</calculatedColumnFormula>
@@ -883,38 +879,38 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
@@ -923,173 +919,173 @@
       <c r="J1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>30</v>
+    <row r="2" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="7">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7">
+        <v>21</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="15" t="s">
-        <v>28</v>
-      </c>
       <c r="K2" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>30</v>
+    <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="7">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="7">
-        <v>4</v>
-      </c>
-      <c r="G3" s="8" t="s">
         <v>7</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="17">
         <f>K3/J3</f>
-        <v>0.90476190476190477</v>
+        <v>1</v>
       </c>
       <c r="J3" s="18">
-        <f>COUNT(B2:B22)</f>
-        <v>21</v>
+        <f>COUNT(B2:B21)</f>
+        <v>20</v>
       </c>
       <c r="K3" s="19">
         <f>COUNTIF(Table4[Status],"Done")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>30</v>
+    <row r="4" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="7">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7">
-        <v>14</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>30</v>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="7">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="9">
-        <v>19</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="9" t="s">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>7</v>
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="H6" s="1"/>
       <c r="J6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="7">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>16</v>
+      <c r="F7" s="7">
+        <v>2</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>7</v>
@@ -1098,200 +1094,200 @@
       <c r="J7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="12">
-        <v>22</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>61</v>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7">
+        <v>9</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>18</v>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7">
-        <v>21</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="H9" s="1"/>
       <c r="J9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>18</v>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="7">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="7">
         <v>1</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7">
+      <c r="G10" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>18</v>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B11" s="7">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="H11" s="1"/>
       <c r="J11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>18</v>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B12" s="7">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="7">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="H12" s="1"/>
       <c r="J12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7">
         <v>18</v>
       </c>
-      <c r="B13" s="7">
-        <v>4</v>
-      </c>
       <c r="C13" s="10" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>12</v>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B14" s="7">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="H14" s="1"/>
       <c r="J14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B15" s="7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>9</v>
@@ -1300,24 +1296,24 @@
         <v>2</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H15" s="1"/>
       <c r="J15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>9</v>
@@ -1326,50 +1322,50 @@
         <v>2</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" s="1"/>
       <c r="J16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H17" s="1"/>
       <c r="J17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="7">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>9</v>
@@ -1378,21 +1374,21 @@
         <v>2</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="H18" s="1"/>
       <c r="J18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>51</v>
@@ -1401,132 +1397,129 @@
         <v>9</v>
       </c>
       <c r="F19" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H19" s="1"/>
       <c r="J19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B20" s="7">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="7">
-        <v>2</v>
+      <c r="F20" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H20" s="1"/>
       <c r="J20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="7">
-        <v>14</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>51</v>
+    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="12">
+        <v>22</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="7">
-        <v>2</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="H21" s="1"/>
       <c r="J21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="7">
+    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="7">
-        <v>1</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="J22" s="4"/>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="J22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="9">
+        <v>19</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="J23" s="5"/>
-      <c r="M23" s="5"/>
-    </row>
-    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="F24" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +1540,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1561,7 +1554,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>